<commit_message>
W2 Excel changes in the for Print
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW2.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW2.xlsx
@@ -19,7 +19,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="Assessment">'[1]Form FS'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Form W2'!$A$1:$Q$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Form W2'!$A$1:$Q$49</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -389,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -718,12 +718,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -866,9 +877,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,6 +904,198 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -923,203 +1123,29 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1159,7 +1185,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7DAE5634-5D8F-40E9-ADBB-2C4FFCA9E28D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DAE5634-5D8F-40E9-ADBB-2C4FFCA9E28D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1209,7 +1235,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{758B2272-2545-44AA-B2DF-8D4582259370}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758B2272-2545-44AA-B2DF-8D4582259370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1288,7 +1314,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6F52695D-B227-4953-BB6B-A50F5660A262}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F52695D-B227-4953-BB6B-A50F5660A262}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1711,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH48"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:P4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48:P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,82 +1760,82 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="77"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
+      <c r="J1" s="139"/>
+      <c r="K1" s="139"/>
+      <c r="L1" s="139"/>
+      <c r="M1" s="139"/>
+      <c r="N1" s="139"/>
+      <c r="O1" s="139"/>
+      <c r="P1" s="139"/>
+      <c r="Q1" s="140"/>
     </row>
     <row r="2" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="80"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="142"/>
+      <c r="Q2" s="143"/>
     </row>
     <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="82"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
+      <c r="Q3" s="145"/>
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="150"/>
-      <c r="N4" s="150"/>
-      <c r="O4" s="150"/>
-      <c r="P4" s="150"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="148"/>
+      <c r="O4" s="148"/>
+      <c r="P4" s="148"/>
       <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1833,16 +1859,16 @@
     </row>
     <row r="6" spans="1:17" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
+      <c r="J6" s="147"/>
+      <c r="K6" s="147"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -1852,25 +1878,25 @@
     </row>
     <row r="7" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="85" t="s">
+      <c r="C7" s="130"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="85"/>
+      <c r="K7" s="130"/>
       <c r="L7" s="28"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
+      <c r="M7" s="136"/>
+      <c r="N7" s="137"/>
+      <c r="O7" s="137"/>
+      <c r="P7" s="137"/>
       <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" ht="1.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1894,25 +1920,25 @@
     </row>
     <row r="9" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="85" t="s">
+      <c r="B9" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="85" t="s">
+      <c r="C9" s="130"/>
+      <c r="D9" s="138"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="85"/>
+      <c r="K9" s="130"/>
       <c r="L9" s="28"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="88"/>
+      <c r="M9" s="136"/>
+      <c r="N9" s="137"/>
+      <c r="O9" s="137"/>
+      <c r="P9" s="137"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1936,25 +1962,25 @@
     </row>
     <row r="11" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="85" t="s">
+      <c r="C11" s="130"/>
+      <c r="D11" s="135"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="85"/>
+      <c r="K11" s="130"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
+      <c r="M11" s="136"/>
+      <c r="N11" s="137"/>
+      <c r="O11" s="137"/>
+      <c r="P11" s="137"/>
       <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1969,94 +1995,94 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
+      <c r="L12" s="132"/>
+      <c r="M12" s="132"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="91"/>
-      <c r="Q12" s="92"/>
+      <c r="P12" s="133"/>
+      <c r="Q12" s="114"/>
     </row>
     <row r="13" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="95"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="96"/>
-      <c r="K13" s="96"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="96"/>
-      <c r="O13" s="96"/>
-      <c r="P13" s="96"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="129"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="85"/>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
-      <c r="F14" s="97"/>
-      <c r="G14" s="97"/>
-      <c r="H14" s="97"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="97"/>
-      <c r="L14" s="97"/>
-      <c r="M14" s="97"/>
-      <c r="N14" s="97"/>
-      <c r="O14" s="97"/>
-      <c r="P14" s="97"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="131"/>
+      <c r="J14" s="131"/>
+      <c r="K14" s="131"/>
+      <c r="L14" s="131"/>
+      <c r="M14" s="131"/>
+      <c r="N14" s="131"/>
+      <c r="O14" s="131"/>
+      <c r="P14" s="131"/>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="85" t="s">
+      <c r="B15" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="97"/>
-      <c r="G15" s="97"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="97"/>
-      <c r="L15" s="97"/>
-      <c r="M15" s="97"/>
-      <c r="N15" s="97"/>
-      <c r="O15" s="97"/>
-      <c r="P15" s="97"/>
+      <c r="C15" s="130"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="131"/>
+      <c r="G15" s="131"/>
+      <c r="H15" s="131"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="131"/>
+      <c r="K15" s="131"/>
+      <c r="L15" s="131"/>
+      <c r="M15" s="131"/>
+      <c r="N15" s="131"/>
+      <c r="O15" s="131"/>
+      <c r="P15" s="131"/>
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:17" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="90"/>
-      <c r="E16" s="90"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="133"/>
+      <c r="I16" s="133"/>
+      <c r="J16" s="133"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
+      <c r="L16" s="132"/>
+      <c r="M16" s="132"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="91"/>
-      <c r="Q16" s="92"/>
+      <c r="P16" s="133"/>
+      <c r="Q16" s="114"/>
     </row>
     <row r="17" spans="1:21" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2079,42 +2105,42 @@
     </row>
     <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="98" t="s">
+      <c r="B18" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
-      <c r="K18" s="98"/>
-      <c r="L18" s="98"/>
-      <c r="M18" s="98"/>
-      <c r="N18" s="98"/>
-      <c r="O18" s="98"/>
-      <c r="P18" s="98"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="134"/>
+      <c r="H18" s="134"/>
+      <c r="I18" s="134"/>
+      <c r="J18" s="134"/>
+      <c r="K18" s="134"/>
+      <c r="L18" s="134"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="134"/>
+      <c r="O18" s="134"/>
+      <c r="P18" s="134"/>
       <c r="Q18" s="16"/>
     </row>
     <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="98"/>
-      <c r="P19" s="98"/>
+      <c r="B19" s="134"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="134"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="134"/>
+      <c r="K19" s="134"/>
+      <c r="L19" s="134"/>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134"/>
+      <c r="O19" s="134"/>
+      <c r="P19" s="134"/>
       <c r="Q19" s="16"/>
       <c r="U19" s="32"/>
     </row>
@@ -2139,67 +2165,67 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="94"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
+      <c r="L21" s="83"/>
+      <c r="M21" s="83"/>
+      <c r="N21" s="83"/>
+      <c r="O21" s="83"/>
+      <c r="P21" s="83"/>
+      <c r="Q21" s="101"/>
     </row>
     <row r="22" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
+      <c r="B22" s="122"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
       <c r="G22" s="37"/>
-      <c r="H22" s="102" t="s">
+      <c r="H22" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="101"/>
-      <c r="M22" s="101"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="101"/>
-      <c r="P22" s="101"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
+      <c r="K22" s="123"/>
+      <c r="L22" s="123"/>
+      <c r="M22" s="123"/>
+      <c r="N22" s="123"/>
+      <c r="O22" s="123"/>
+      <c r="P22" s="123"/>
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="103" t="s">
+      <c r="A23" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="104"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="105"/>
-      <c r="N23" s="105"/>
-      <c r="O23" s="105"/>
-      <c r="P23" s="105"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="127"/>
+      <c r="L23" s="127"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="127"/>
+      <c r="O23" s="127"/>
+      <c r="P23" s="127"/>
       <c r="Q23" s="38"/>
     </row>
     <row r="24" spans="1:21" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2223,24 +2249,24 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="93" t="s">
+      <c r="B25" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
-      <c r="J25" s="93"/>
-      <c r="K25" s="93"/>
-      <c r="L25" s="93"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
-      <c r="O25" s="93"/>
-      <c r="P25" s="93"/>
-      <c r="Q25" s="94"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="83"/>
+      <c r="M25" s="83"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="83"/>
+      <c r="P25" s="83"/>
+      <c r="Q25" s="101"/>
     </row>
     <row r="26" spans="1:21" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
@@ -2249,329 +2275,329 @@
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
-      <c r="E26" s="107" t="s">
+      <c r="E26" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="107"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="107"/>
-      <c r="P26" s="107"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="102"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="102"/>
       <c r="Q26" s="43"/>
     </row>
     <row r="27" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="108"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="111" t="s">
+      <c r="C27" s="103"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="104"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="112"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="112"/>
-      <c r="M27" s="112"/>
-      <c r="N27" s="112"/>
-      <c r="O27" s="112"/>
-      <c r="P27" s="112"/>
-      <c r="Q27" s="117"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="107"/>
+      <c r="N27" s="107"/>
+      <c r="O27" s="107"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="112"/>
     </row>
     <row r="28" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
-      <c r="B28" s="108" t="s">
+      <c r="B28" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="108"/>
-      <c r="D28" s="108"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="110"/>
-      <c r="G28" s="110"/>
-      <c r="H28" s="110"/>
-      <c r="I28" s="113"/>
-      <c r="J28" s="114"/>
-      <c r="K28" s="114"/>
-      <c r="L28" s="114"/>
-      <c r="M28" s="114"/>
-      <c r="N28" s="114"/>
-      <c r="O28" s="114"/>
-      <c r="P28" s="114"/>
-      <c r="Q28" s="118"/>
+      <c r="C28" s="103"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="105"/>
+      <c r="G28" s="105"/>
+      <c r="H28" s="105"/>
+      <c r="I28" s="108"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="109"/>
+      <c r="M28" s="109"/>
+      <c r="N28" s="109"/>
+      <c r="O28" s="109"/>
+      <c r="P28" s="109"/>
+      <c r="Q28" s="113"/>
     </row>
     <row r="29" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
-      <c r="B29" s="119" t="s">
+      <c r="B29" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="120"/>
-      <c r="G29" s="121" t="s">
+      <c r="C29" s="115"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="121"/>
-      <c r="I29" s="115"/>
-      <c r="J29" s="116"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="116"/>
-      <c r="N29" s="116"/>
-      <c r="O29" s="116"/>
-      <c r="P29" s="116"/>
-      <c r="Q29" s="92"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="111"/>
+      <c r="N29" s="111"/>
+      <c r="O29" s="111"/>
+      <c r="P29" s="111"/>
+      <c r="Q29" s="114"/>
     </row>
     <row r="30" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="93"/>
-      <c r="D30" s="93"/>
-      <c r="E30" s="93"/>
-      <c r="F30" s="93"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="93"/>
-      <c r="M30" s="93"/>
-      <c r="N30" s="93"/>
-      <c r="O30" s="93"/>
-      <c r="P30" s="93"/>
-      <c r="Q30" s="94"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="83"/>
+      <c r="L30" s="83"/>
+      <c r="M30" s="83"/>
+      <c r="N30" s="83"/>
+      <c r="O30" s="83"/>
+      <c r="P30" s="83"/>
+      <c r="Q30" s="101"/>
     </row>
     <row r="31" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="122" t="s">
+      <c r="A31" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="123"/>
-      <c r="C31" s="123"/>
-      <c r="D31" s="123"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="123"/>
-      <c r="H31" s="123"/>
-      <c r="I31" s="123"/>
-      <c r="J31" s="123"/>
-      <c r="K31" s="123"/>
-      <c r="L31" s="123"/>
-      <c r="M31" s="123"/>
-      <c r="N31" s="123"/>
-      <c r="O31" s="123"/>
-      <c r="P31" s="123"/>
-      <c r="Q31" s="124"/>
+      <c r="B31" s="119"/>
+      <c r="C31" s="119"/>
+      <c r="D31" s="119"/>
+      <c r="E31" s="119"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="119"/>
+      <c r="H31" s="119"/>
+      <c r="I31" s="119"/>
+      <c r="J31" s="119"/>
+      <c r="K31" s="119"/>
+      <c r="L31" s="119"/>
+      <c r="M31" s="119"/>
+      <c r="N31" s="119"/>
+      <c r="O31" s="119"/>
+      <c r="P31" s="119"/>
+      <c r="Q31" s="120"/>
     </row>
     <row r="32" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
-      <c r="B32" s="144"/>
-      <c r="C32" s="144"/>
-      <c r="D32" s="144"/>
-      <c r="E32" s="144"/>
-      <c r="F32" s="144"/>
-      <c r="G32" s="144"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="144"/>
-      <c r="J32" s="144"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="144"/>
-      <c r="M32" s="144"/>
-      <c r="N32" s="144"/>
-      <c r="O32" s="144"/>
-      <c r="P32" s="144"/>
-      <c r="Q32" s="74"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="99"/>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
+      <c r="J32" s="99"/>
+      <c r="K32" s="99"/>
+      <c r="L32" s="99"/>
+      <c r="M32" s="99"/>
+      <c r="N32" s="99"/>
+      <c r="O32" s="99"/>
+      <c r="P32" s="99"/>
+      <c r="Q32" s="73"/>
     </row>
     <row r="33" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
-      <c r="B33" s="144"/>
-      <c r="C33" s="144"/>
-      <c r="D33" s="144"/>
-      <c r="E33" s="144"/>
-      <c r="F33" s="144"/>
-      <c r="G33" s="144"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="144"/>
-      <c r="J33" s="144"/>
-      <c r="K33" s="144"/>
-      <c r="L33" s="144"/>
-      <c r="M33" s="144"/>
-      <c r="N33" s="144"/>
-      <c r="O33" s="144"/>
-      <c r="P33" s="144"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="72"/>
-      <c r="S33" s="106"/>
-      <c r="T33" s="106"/>
-      <c r="U33" s="106"/>
-      <c r="V33" s="106"/>
-      <c r="W33" s="106"/>
-      <c r="X33" s="106"/>
-      <c r="Y33" s="106"/>
-      <c r="Z33" s="106"/>
-      <c r="AA33" s="106"/>
-      <c r="AB33" s="106"/>
-      <c r="AC33" s="106"/>
-      <c r="AD33" s="106"/>
-      <c r="AE33" s="106"/>
-      <c r="AF33" s="106"/>
-      <c r="AG33" s="106"/>
-      <c r="AH33" s="72"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="99"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="99"/>
+      <c r="K33" s="99"/>
+      <c r="L33" s="99"/>
+      <c r="M33" s="99"/>
+      <c r="N33" s="99"/>
+      <c r="O33" s="99"/>
+      <c r="P33" s="99"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="71"/>
+      <c r="S33" s="82"/>
+      <c r="T33" s="82"/>
+      <c r="U33" s="82"/>
+      <c r="V33" s="82"/>
+      <c r="W33" s="82"/>
+      <c r="X33" s="82"/>
+      <c r="Y33" s="82"/>
+      <c r="Z33" s="82"/>
+      <c r="AA33" s="82"/>
+      <c r="AB33" s="82"/>
+      <c r="AC33" s="82"/>
+      <c r="AD33" s="82"/>
+      <c r="AE33" s="82"/>
+      <c r="AF33" s="82"/>
+      <c r="AG33" s="82"/>
+      <c r="AH33" s="71"/>
     </row>
     <row r="34" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-      <c r="B34" s="144"/>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="144"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="144"/>
-      <c r="J34" s="144"/>
-      <c r="K34" s="144"/>
-      <c r="L34" s="144"/>
-      <c r="M34" s="144"/>
-      <c r="N34" s="144"/>
-      <c r="O34" s="144"/>
-      <c r="P34" s="144"/>
-      <c r="Q34" s="74"/>
-      <c r="R34" s="72"/>
-      <c r="S34" s="106"/>
-      <c r="T34" s="106"/>
-      <c r="U34" s="106"/>
-      <c r="V34" s="106"/>
-      <c r="W34" s="106"/>
-      <c r="X34" s="106"/>
-      <c r="Y34" s="106"/>
-      <c r="Z34" s="106"/>
-      <c r="AA34" s="106"/>
-      <c r="AB34" s="106"/>
-      <c r="AC34" s="106"/>
-      <c r="AD34" s="106"/>
-      <c r="AE34" s="106"/>
-      <c r="AF34" s="106"/>
-      <c r="AG34" s="106"/>
-      <c r="AH34" s="72"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="99"/>
+      <c r="F34" s="99"/>
+      <c r="G34" s="99"/>
+      <c r="H34" s="99"/>
+      <c r="I34" s="99"/>
+      <c r="J34" s="99"/>
+      <c r="K34" s="99"/>
+      <c r="L34" s="99"/>
+      <c r="M34" s="99"/>
+      <c r="N34" s="99"/>
+      <c r="O34" s="99"/>
+      <c r="P34" s="99"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="71"/>
+      <c r="S34" s="82"/>
+      <c r="T34" s="82"/>
+      <c r="U34" s="82"/>
+      <c r="V34" s="82"/>
+      <c r="W34" s="82"/>
+      <c r="X34" s="82"/>
+      <c r="Y34" s="82"/>
+      <c r="Z34" s="82"/>
+      <c r="AA34" s="82"/>
+      <c r="AB34" s="82"/>
+      <c r="AC34" s="82"/>
+      <c r="AD34" s="82"/>
+      <c r="AE34" s="82"/>
+      <c r="AF34" s="82"/>
+      <c r="AG34" s="82"/>
+      <c r="AH34" s="71"/>
     </row>
     <row r="35" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="144"/>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="144"/>
-      <c r="J35" s="144"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="144"/>
-      <c r="M35" s="144"/>
-      <c r="N35" s="144"/>
-      <c r="O35" s="144"/>
-      <c r="P35" s="144"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="72"/>
-      <c r="S35" s="106"/>
-      <c r="T35" s="106"/>
-      <c r="U35" s="106"/>
-      <c r="V35" s="106"/>
-      <c r="W35" s="106"/>
-      <c r="X35" s="106"/>
-      <c r="Y35" s="106"/>
-      <c r="Z35" s="106"/>
-      <c r="AA35" s="106"/>
-      <c r="AB35" s="106"/>
-      <c r="AC35" s="106"/>
-      <c r="AD35" s="106"/>
-      <c r="AE35" s="106"/>
-      <c r="AF35" s="106"/>
-      <c r="AG35" s="106"/>
-      <c r="AH35" s="72"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="99"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="99"/>
+      <c r="K35" s="99"/>
+      <c r="L35" s="99"/>
+      <c r="M35" s="99"/>
+      <c r="N35" s="99"/>
+      <c r="O35" s="99"/>
+      <c r="P35" s="99"/>
+      <c r="Q35" s="73"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="82"/>
+      <c r="T35" s="82"/>
+      <c r="U35" s="82"/>
+      <c r="V35" s="82"/>
+      <c r="W35" s="82"/>
+      <c r="X35" s="82"/>
+      <c r="Y35" s="82"/>
+      <c r="Z35" s="82"/>
+      <c r="AA35" s="82"/>
+      <c r="AB35" s="82"/>
+      <c r="AC35" s="82"/>
+      <c r="AD35" s="82"/>
+      <c r="AE35" s="82"/>
+      <c r="AF35" s="82"/>
+      <c r="AG35" s="82"/>
+      <c r="AH35" s="71"/>
     </row>
     <row r="36" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
-      <c r="B36" s="144"/>
-      <c r="C36" s="144"/>
-      <c r="D36" s="144"/>
-      <c r="E36" s="144"/>
-      <c r="F36" s="144"/>
-      <c r="G36" s="144"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
-      <c r="J36" s="144"/>
-      <c r="K36" s="144"/>
-      <c r="L36" s="144"/>
-      <c r="M36" s="144"/>
-      <c r="N36" s="144"/>
-      <c r="O36" s="144"/>
-      <c r="P36" s="144"/>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="72"/>
-      <c r="S36" s="106"/>
-      <c r="T36" s="106"/>
-      <c r="U36" s="106"/>
-      <c r="V36" s="106"/>
-      <c r="W36" s="106"/>
-      <c r="X36" s="106"/>
-      <c r="Y36" s="106"/>
-      <c r="Z36" s="106"/>
-      <c r="AA36" s="106"/>
-      <c r="AB36" s="106"/>
-      <c r="AC36" s="106"/>
-      <c r="AD36" s="106"/>
-      <c r="AE36" s="106"/>
-      <c r="AF36" s="106"/>
-      <c r="AG36" s="106"/>
-      <c r="AH36" s="72"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="99"/>
+      <c r="L36" s="99"/>
+      <c r="M36" s="99"/>
+      <c r="N36" s="99"/>
+      <c r="O36" s="99"/>
+      <c r="P36" s="99"/>
+      <c r="Q36" s="73"/>
+      <c r="R36" s="71"/>
+      <c r="S36" s="82"/>
+      <c r="T36" s="82"/>
+      <c r="U36" s="82"/>
+      <c r="V36" s="82"/>
+      <c r="W36" s="82"/>
+      <c r="X36" s="82"/>
+      <c r="Y36" s="82"/>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="82"/>
+      <c r="AB36" s="82"/>
+      <c r="AC36" s="82"/>
+      <c r="AD36" s="82"/>
+      <c r="AE36" s="82"/>
+      <c r="AF36" s="82"/>
+      <c r="AG36" s="82"/>
+      <c r="AH36" s="71"/>
     </row>
     <row r="37" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
-      <c r="B37" s="145"/>
-      <c r="C37" s="145"/>
-      <c r="D37" s="145"/>
-      <c r="E37" s="145"/>
-      <c r="F37" s="145"/>
-      <c r="G37" s="145"/>
-      <c r="H37" s="145"/>
-      <c r="I37" s="145"/>
-      <c r="J37" s="145"/>
-      <c r="K37" s="145"/>
-      <c r="L37" s="145"/>
-      <c r="M37" s="145"/>
-      <c r="N37" s="145"/>
-      <c r="O37" s="145"/>
-      <c r="P37" s="145"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="106"/>
-      <c r="T37" s="106"/>
-      <c r="U37" s="106"/>
-      <c r="V37" s="106"/>
-      <c r="W37" s="106"/>
-      <c r="X37" s="106"/>
-      <c r="Y37" s="106"/>
-      <c r="Z37" s="106"/>
-      <c r="AA37" s="106"/>
-      <c r="AB37" s="106"/>
-      <c r="AC37" s="106"/>
-      <c r="AD37" s="106"/>
-      <c r="AE37" s="106"/>
-      <c r="AF37" s="106"/>
-      <c r="AG37" s="106"/>
-      <c r="AH37" s="72"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="100"/>
+      <c r="I37" s="100"/>
+      <c r="J37" s="100"/>
+      <c r="K37" s="100"/>
+      <c r="L37" s="100"/>
+      <c r="M37" s="100"/>
+      <c r="N37" s="100"/>
+      <c r="O37" s="100"/>
+      <c r="P37" s="100"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="82"/>
+      <c r="T37" s="82"/>
+      <c r="U37" s="82"/>
+      <c r="V37" s="82"/>
+      <c r="W37" s="82"/>
+      <c r="X37" s="82"/>
+      <c r="Y37" s="82"/>
+      <c r="Z37" s="82"/>
+      <c r="AA37" s="82"/>
+      <c r="AB37" s="82"/>
+      <c r="AC37" s="82"/>
+      <c r="AD37" s="82"/>
+      <c r="AE37" s="82"/>
+      <c r="AF37" s="82"/>
+      <c r="AG37" s="82"/>
+      <c r="AH37" s="71"/>
     </row>
     <row r="38" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
@@ -2590,79 +2616,79 @@
       <c r="N38" s="48"/>
       <c r="O38" s="48"/>
       <c r="P38" s="48"/>
-      <c r="Q38" s="75"/>
-      <c r="R38" s="72"/>
-      <c r="S38" s="73"/>
-      <c r="T38" s="72"/>
-      <c r="U38" s="72"/>
-      <c r="V38" s="72"/>
-      <c r="W38" s="72"/>
-      <c r="X38" s="72"/>
-      <c r="Y38" s="72"/>
-      <c r="Z38" s="72"/>
-      <c r="AA38" s="72"/>
-      <c r="AB38" s="72"/>
-      <c r="AC38" s="72"/>
-      <c r="AD38" s="72"/>
-      <c r="AE38" s="72"/>
-      <c r="AF38" s="72"/>
-      <c r="AG38" s="72"/>
-      <c r="AH38" s="72"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="71"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="71"/>
+      <c r="U38" s="71"/>
+      <c r="V38" s="71"/>
+      <c r="W38" s="71"/>
+      <c r="X38" s="71"/>
+      <c r="Y38" s="71"/>
+      <c r="Z38" s="71"/>
+      <c r="AA38" s="71"/>
+      <c r="AB38" s="71"/>
+      <c r="AC38" s="71"/>
+      <c r="AD38" s="71"/>
+      <c r="AE38" s="71"/>
+      <c r="AF38" s="71"/>
+      <c r="AG38" s="71"/>
+      <c r="AH38" s="71"/>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="93" t="s">
+      <c r="B39" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
-      <c r="O39" s="93"/>
-      <c r="P39" s="93"/>
-      <c r="Q39" s="71"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="72"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
-      <c r="AA39" s="72"/>
-      <c r="AB39" s="72"/>
-      <c r="AC39" s="72"/>
-      <c r="AD39" s="72"/>
-      <c r="AE39" s="72"/>
-      <c r="AF39" s="72"/>
-      <c r="AG39" s="72"/>
-      <c r="AH39" s="72"/>
+      <c r="C39" s="83"/>
+      <c r="D39" s="83"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="83"/>
+      <c r="J39" s="83"/>
+      <c r="K39" s="83"/>
+      <c r="L39" s="83"/>
+      <c r="M39" s="83"/>
+      <c r="N39" s="83"/>
+      <c r="O39" s="83"/>
+      <c r="P39" s="83"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="71"/>
+      <c r="S39" s="71"/>
+      <c r="T39" s="71"/>
+      <c r="U39" s="71"/>
+      <c r="V39" s="71"/>
+      <c r="W39" s="71"/>
+      <c r="X39" s="71"/>
+      <c r="Y39" s="71"/>
+      <c r="Z39" s="71"/>
+      <c r="AA39" s="71"/>
+      <c r="AB39" s="71"/>
+      <c r="AC39" s="71"/>
+      <c r="AD39" s="71"/>
+      <c r="AE39" s="71"/>
+      <c r="AF39" s="71"/>
+      <c r="AG39" s="71"/>
+      <c r="AH39" s="71"/>
     </row>
     <row r="40" spans="1:34" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
-      <c r="B40" s="129" t="s">
+      <c r="B40" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="131"/>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="131"/>
-      <c r="G40" s="131"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
       <c r="H40" s="49"/>
-      <c r="I40" s="134" t="s">
+      <c r="I40" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="J40" s="135"/>
-      <c r="K40" s="135"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
       <c r="L40" s="49"/>
       <c r="M40" s="49"/>
       <c r="N40" s="49"/>
@@ -2672,16 +2698,16 @@
     </row>
     <row r="41" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="132"/>
-      <c r="G41" s="132"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="136"/>
-      <c r="J41" s="137"/>
-      <c r="K41" s="137"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="92"/>
+      <c r="K41" s="92"/>
       <c r="L41" s="52"/>
       <c r="M41" s="52"/>
       <c r="N41" s="52"/>
@@ -2691,12 +2717,12 @@
     </row>
     <row r="42" spans="1:34" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="133"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="133"/>
-      <c r="F42" s="133"/>
-      <c r="G42" s="133"/>
+      <c r="B42" s="85"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="88"/>
       <c r="H42" s="4"/>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
@@ -2726,35 +2752,35 @@
       <c r="O43" s="58"/>
       <c r="P43" s="58"/>
       <c r="Q43" s="56"/>
-      <c r="R43" s="138"/>
-      <c r="S43" s="139"/>
-      <c r="T43" s="139"/>
-      <c r="U43" s="139"/>
+      <c r="R43" s="93"/>
+      <c r="S43" s="94"/>
+      <c r="T43" s="94"/>
+      <c r="U43" s="94"/>
     </row>
     <row r="44" spans="1:34" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
-      <c r="B44" s="137" t="s">
+      <c r="B44" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="137"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="142"/>
-      <c r="J44" s="143"/>
-      <c r="K44" s="143"/>
-      <c r="L44" s="143"/>
-      <c r="M44" s="143"/>
-      <c r="N44" s="143"/>
-      <c r="O44" s="127"/>
-      <c r="P44" s="127"/>
-      <c r="Q44" s="128"/>
-      <c r="R44" s="138"/>
-      <c r="S44" s="139"/>
-      <c r="T44" s="139"/>
-      <c r="U44" s="139"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="95"/>
+      <c r="F44" s="95"/>
+      <c r="G44" s="95"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="98"/>
+      <c r="K44" s="98"/>
+      <c r="L44" s="98"/>
+      <c r="M44" s="98"/>
+      <c r="N44" s="98"/>
+      <c r="O44" s="80"/>
+      <c r="P44" s="80"/>
+      <c r="Q44" s="81"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="94"/>
+      <c r="T44" s="94"/>
+      <c r="U44" s="94"/>
     </row>
     <row r="45" spans="1:34" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
@@ -2762,91 +2788,184 @@
       <c r="C45" s="60"/>
       <c r="D45" s="61"/>
       <c r="E45" s="61"/>
-      <c r="F45" s="125"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="125"/>
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="78"/>
       <c r="I45" s="62"/>
-      <c r="J45" s="126"/>
-      <c r="K45" s="126"/>
-      <c r="L45" s="126"/>
-      <c r="M45" s="126"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
       <c r="N45" s="63"/>
-      <c r="O45" s="127"/>
-      <c r="P45" s="127"/>
-      <c r="Q45" s="128"/>
-    </row>
-    <row r="46" spans="1:34" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="81"/>
+    </row>
+    <row r="46" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="149" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="146"/>
-      <c r="D46" s="146"/>
-      <c r="E46" s="146"/>
-      <c r="F46" s="146"/>
-      <c r="G46" s="146"/>
-      <c r="H46" s="146"/>
-      <c r="I46" s="147" t="s">
+      <c r="C46" s="154"/>
+      <c r="D46" s="154"/>
+      <c r="E46" s="154"/>
+      <c r="F46" s="154"/>
+      <c r="G46" s="154"/>
+      <c r="H46" s="155"/>
+      <c r="I46" s="152" t="s">
         <v>31</v>
       </c>
-      <c r="J46" s="148"/>
-      <c r="K46" s="146"/>
-      <c r="L46" s="146"/>
-      <c r="M46" s="146"/>
-      <c r="N46" s="146"/>
-      <c r="O46" s="146"/>
-      <c r="P46" s="146"/>
-      <c r="Q46" s="65"/>
+      <c r="J46" s="152"/>
+      <c r="K46" s="153"/>
+      <c r="L46" s="153"/>
+      <c r="M46" s="153"/>
+      <c r="N46" s="153"/>
+      <c r="O46" s="153"/>
+      <c r="P46" s="153"/>
+      <c r="Q46" s="64"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A47" s="66"/>
-      <c r="B47" s="67"/>
-      <c r="C47" s="149" t="s">
+      <c r="A47" s="59"/>
+      <c r="B47" s="149"/>
+      <c r="C47" s="153"/>
+      <c r="D47" s="153"/>
+      <c r="E47" s="153"/>
+      <c r="F47" s="153"/>
+      <c r="G47" s="153"/>
+      <c r="H47" s="96"/>
+      <c r="I47" s="151"/>
+      <c r="J47" s="152"/>
+      <c r="K47" s="153"/>
+      <c r="L47" s="153"/>
+      <c r="M47" s="153"/>
+      <c r="N47" s="153"/>
+      <c r="O47" s="153"/>
+      <c r="P47" s="153"/>
+      <c r="Q47" s="75"/>
+    </row>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A48" s="59"/>
+      <c r="B48" s="149"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+      <c r="H48" s="150"/>
+      <c r="I48" s="151"/>
+      <c r="J48" s="152"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="76"/>
+      <c r="P48" s="76"/>
+      <c r="Q48" s="75"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="65"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="149"/>
-      <c r="E47" s="149"/>
-      <c r="F47" s="149"/>
-      <c r="G47" s="149"/>
-      <c r="H47" s="149"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="69"/>
-      <c r="K47" s="149" t="s">
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="77"/>
+      <c r="G49" s="77"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="L47" s="149"/>
-      <c r="M47" s="149"/>
-      <c r="N47" s="149"/>
-      <c r="O47" s="149"/>
-      <c r="P47" s="149"/>
-      <c r="Q47" s="70"/>
-    </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A48" s="57"/>
-      <c r="B48" s="57"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="57"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
+      <c r="L49" s="77"/>
+      <c r="M49" s="77"/>
+      <c r="N49" s="77"/>
+      <c r="O49" s="77"/>
+      <c r="P49" s="77"/>
+      <c r="Q49" s="69"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="57"/>
+      <c r="B50" s="57"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="32"/>
+      <c r="N50" s="32"/>
+      <c r="O50" s="32"/>
+      <c r="P50" s="32"/>
+      <c r="Q50" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:P46"/>
+  <mergeCells count="80">
+    <mergeCell ref="B46:B48"/>
     <mergeCell ref="C47:H47"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="I46:J48"/>
+    <mergeCell ref="K48:P48"/>
     <mergeCell ref="K47:P47"/>
+    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="D3:Q3"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="B21:Q21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:P13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:P14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:P15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="B18:P19"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:P22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:P23"/>
+    <mergeCell ref="S36:AG36"/>
+    <mergeCell ref="S33:AG33"/>
+    <mergeCell ref="B25:Q25"/>
+    <mergeCell ref="E26:P26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="I27:P29"/>
+    <mergeCell ref="Q27:Q29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B30:Q30"/>
+    <mergeCell ref="A31:Q31"/>
     <mergeCell ref="F45:H45"/>
     <mergeCell ref="J45:M45"/>
     <mergeCell ref="O45:Q45"/>
@@ -2863,60 +2982,10 @@
     <mergeCell ref="B32:P37"/>
     <mergeCell ref="S34:AG34"/>
     <mergeCell ref="S35:AG35"/>
-    <mergeCell ref="S36:AG36"/>
-    <mergeCell ref="S33:AG33"/>
-    <mergeCell ref="B25:Q25"/>
-    <mergeCell ref="E26:P26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="I27:P29"/>
-    <mergeCell ref="Q27:Q29"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B30:Q30"/>
-    <mergeCell ref="A31:Q31"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:P22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:P23"/>
-    <mergeCell ref="B21:Q21"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:P13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:P14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:P15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="B18:P19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="D1:Q1"/>
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="D3:Q3"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="K46:P46"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="K49:P49"/>
   </mergeCells>
   <pageMargins left="0.9055118110236221" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
@@ -2934,12 +3003,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -3156,6 +3219,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
   <ds:schemaRefs>
@@ -3165,23 +3234,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3198,4 +3250,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0930cf9b-719b-4120-8db4-f84070340397"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="4e744003-367c-4be8-bc40-2385cb622540"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
iw forms user acess
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW2.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormW2.xlsx
@@ -734,7 +734,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -907,245 +907,239 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1739,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48:P48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,82 +1754,82 @@
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="139"/>
-      <c r="O1" s="139"/>
-      <c r="P1" s="139"/>
-      <c r="Q1" s="140"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="138"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
+      <c r="P1" s="138"/>
+      <c r="Q1" s="139"/>
     </row>
     <row r="2" spans="1:17" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="141" t="s">
+      <c r="D2" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
-      <c r="O2" s="142"/>
-      <c r="P2" s="142"/>
-      <c r="Q2" s="143"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141"/>
+      <c r="O2" s="141"/>
+      <c r="P2" s="141"/>
+      <c r="Q2" s="142"/>
     </row>
     <row r="3" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="144" t="s">
+      <c r="D3" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="144"/>
-      <c r="P3" s="144"/>
-      <c r="Q3" s="145"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="143"/>
+      <c r="P3" s="143"/>
+      <c r="Q3" s="144"/>
     </row>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="146"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="148"/>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
+      <c r="E4" s="145"/>
+      <c r="F4" s="145"/>
+      <c r="G4" s="145"/>
+      <c r="H4" s="145"/>
+      <c r="I4" s="145"/>
+      <c r="J4" s="145"/>
+      <c r="K4" s="145"/>
+      <c r="L4" s="145"/>
+      <c r="M4" s="147"/>
+      <c r="N4" s="147"/>
+      <c r="O4" s="147"/>
+      <c r="P4" s="147"/>
       <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1859,16 +1853,16 @@
     </row>
     <row r="6" spans="1:17" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="147"/>
-      <c r="C6" s="147"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="146"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="147"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -1878,25 +1872,25 @@
     </row>
     <row r="7" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="130" t="s">
+      <c r="C7" s="129"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="130"/>
+      <c r="K7" s="129"/>
       <c r="L7" s="28"/>
-      <c r="M7" s="136"/>
-      <c r="N7" s="137"/>
-      <c r="O7" s="137"/>
-      <c r="P7" s="137"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
       <c r="Q7" s="13"/>
     </row>
     <row r="8" spans="1:17" ht="1.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1920,25 +1914,25 @@
     </row>
     <row r="9" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
-      <c r="B9" s="130" t="s">
+      <c r="B9" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="130"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="138"/>
-      <c r="F9" s="138"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="138"/>
-      <c r="I9" s="138"/>
-      <c r="J9" s="130" t="s">
+      <c r="C9" s="129"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="J9" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="130"/>
+      <c r="K9" s="129"/>
       <c r="L9" s="28"/>
-      <c r="M9" s="136"/>
-      <c r="N9" s="137"/>
-      <c r="O9" s="137"/>
-      <c r="P9" s="137"/>
+      <c r="M9" s="135"/>
+      <c r="N9" s="136"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
       <c r="Q9" s="13"/>
     </row>
     <row r="10" spans="1:17" ht="2.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -1962,25 +1956,25 @@
     </row>
     <row r="11" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
-      <c r="B11" s="130" t="s">
+      <c r="B11" s="129" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="130"/>
-      <c r="D11" s="135"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="135"/>
-      <c r="I11" s="135"/>
-      <c r="J11" s="130" t="s">
+      <c r="C11" s="129"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="134"/>
+      <c r="I11" s="134"/>
+      <c r="J11" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="130"/>
+      <c r="K11" s="129"/>
       <c r="L11" s="28"/>
-      <c r="M11" s="136"/>
-      <c r="N11" s="137"/>
-      <c r="O11" s="137"/>
-      <c r="P11" s="137"/>
+      <c r="M11" s="135"/>
+      <c r="N11" s="136"/>
+      <c r="O11" s="136"/>
+      <c r="P11" s="136"/>
       <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1995,94 +1989,94 @@
       <c r="I12" s="15"/>
       <c r="J12" s="15"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="132"/>
-      <c r="M12" s="132"/>
+      <c r="L12" s="131"/>
+      <c r="M12" s="131"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="133"/>
-      <c r="Q12" s="114"/>
+      <c r="P12" s="132"/>
+      <c r="Q12" s="113"/>
     </row>
     <row r="13" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="128"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
+      <c r="C13" s="127"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="128"/>
+      <c r="F13" s="128"/>
+      <c r="G13" s="128"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="128"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="128"/>
+      <c r="M13" s="128"/>
+      <c r="N13" s="128"/>
+      <c r="O13" s="128"/>
+      <c r="P13" s="128"/>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="130" t="s">
+      <c r="B14" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="130"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="131"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="131"/>
-      <c r="H14" s="131"/>
-      <c r="I14" s="131"/>
-      <c r="J14" s="131"/>
-      <c r="K14" s="131"/>
-      <c r="L14" s="131"/>
-      <c r="M14" s="131"/>
-      <c r="N14" s="131"/>
-      <c r="O14" s="131"/>
-      <c r="P14" s="131"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="130"/>
+      <c r="L14" s="130"/>
+      <c r="M14" s="130"/>
+      <c r="N14" s="130"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
       <c r="Q14" s="13"/>
     </row>
     <row r="15" spans="1:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="130" t="s">
+      <c r="B15" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="130"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="131"/>
-      <c r="J15" s="131"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="131"/>
-      <c r="N15" s="131"/>
-      <c r="O15" s="131"/>
-      <c r="P15" s="131"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="130"/>
+      <c r="L15" s="130"/>
+      <c r="M15" s="130"/>
+      <c r="N15" s="130"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
       <c r="Q15" s="13"/>
     </row>
     <row r="16" spans="1:17" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="132"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="132"/>
-      <c r="M16" s="132"/>
+      <c r="L16" s="131"/>
+      <c r="M16" s="131"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="114"/>
+      <c r="P16" s="132"/>
+      <c r="Q16" s="113"/>
     </row>
     <row r="17" spans="1:21" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -2105,42 +2099,42 @@
     </row>
     <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="134" t="s">
+      <c r="B18" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="134"/>
-      <c r="D18" s="134"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
-      <c r="K18" s="134"/>
-      <c r="L18" s="134"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="134"/>
-      <c r="O18" s="134"/>
-      <c r="P18" s="134"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="133"/>
+      <c r="I18" s="133"/>
+      <c r="J18" s="133"/>
+      <c r="K18" s="133"/>
+      <c r="L18" s="133"/>
+      <c r="M18" s="133"/>
+      <c r="N18" s="133"/>
+      <c r="O18" s="133"/>
+      <c r="P18" s="133"/>
       <c r="Q18" s="16"/>
     </row>
     <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="134"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134"/>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
-      <c r="J19" s="134"/>
-      <c r="K19" s="134"/>
-      <c r="L19" s="134"/>
-      <c r="M19" s="134"/>
-      <c r="N19" s="134"/>
-      <c r="O19" s="134"/>
-      <c r="P19" s="134"/>
+      <c r="B19" s="133"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="133"/>
+      <c r="H19" s="133"/>
+      <c r="I19" s="133"/>
+      <c r="J19" s="133"/>
+      <c r="K19" s="133"/>
+      <c r="L19" s="133"/>
+      <c r="M19" s="133"/>
+      <c r="N19" s="133"/>
+      <c r="O19" s="133"/>
+      <c r="P19" s="133"/>
       <c r="Q19" s="16"/>
       <c r="U19" s="32"/>
     </row>
@@ -2165,67 +2159,67 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="83"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="83"/>
-      <c r="N21" s="83"/>
-      <c r="O21" s="83"/>
-      <c r="P21" s="83"/>
-      <c r="Q21" s="101"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="82"/>
+      <c r="M21" s="82"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="82"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="100"/>
     </row>
     <row r="22" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="121" t="s">
+      <c r="A22" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="122"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="122"/>
+      <c r="E22" s="122"/>
+      <c r="F22" s="122"/>
       <c r="G22" s="37"/>
-      <c r="H22" s="124" t="s">
+      <c r="H22" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="124"/>
-      <c r="J22" s="124"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="123"/>
-      <c r="M22" s="123"/>
-      <c r="N22" s="123"/>
-      <c r="O22" s="123"/>
-      <c r="P22" s="123"/>
+      <c r="I22" s="123"/>
+      <c r="J22" s="123"/>
+      <c r="K22" s="122"/>
+      <c r="L22" s="122"/>
+      <c r="M22" s="122"/>
+      <c r="N22" s="122"/>
+      <c r="O22" s="122"/>
+      <c r="P22" s="122"/>
       <c r="Q22" s="18"/>
     </row>
     <row r="23" spans="1:21" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="125" t="s">
+      <c r="A23" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="126"/>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="127"/>
-      <c r="J23" s="127"/>
-      <c r="K23" s="127"/>
-      <c r="L23" s="127"/>
-      <c r="M23" s="127"/>
-      <c r="N23" s="127"/>
-      <c r="O23" s="127"/>
-      <c r="P23" s="127"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="126"/>
+      <c r="K23" s="126"/>
+      <c r="L23" s="126"/>
+      <c r="M23" s="126"/>
+      <c r="N23" s="126"/>
+      <c r="O23" s="126"/>
+      <c r="P23" s="126"/>
       <c r="Q23" s="38"/>
     </row>
     <row r="24" spans="1:21" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2249,24 +2243,24 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="83"/>
-      <c r="I25" s="83"/>
-      <c r="J25" s="83"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="83"/>
-      <c r="M25" s="83"/>
-      <c r="N25" s="83"/>
-      <c r="O25" s="83"/>
-      <c r="P25" s="83"/>
-      <c r="Q25" s="101"/>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="82"/>
+      <c r="P25" s="82"/>
+      <c r="Q25" s="100"/>
     </row>
     <row r="26" spans="1:21" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
@@ -2275,328 +2269,328 @@
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="42"/>
-      <c r="E26" s="102" t="s">
+      <c r="E26" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="102"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="102"/>
-      <c r="I26" s="102"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="102"/>
-      <c r="L26" s="102"/>
-      <c r="M26" s="102"/>
-      <c r="N26" s="102"/>
-      <c r="O26" s="102"/>
-      <c r="P26" s="102"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="101"/>
+      <c r="I26" s="101"/>
+      <c r="J26" s="101"/>
+      <c r="K26" s="101"/>
+      <c r="L26" s="101"/>
+      <c r="M26" s="101"/>
+      <c r="N26" s="101"/>
+      <c r="O26" s="101"/>
+      <c r="P26" s="101"/>
       <c r="Q26" s="43"/>
     </row>
     <row r="27" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="103"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="106" t="s">
+      <c r="C27" s="102"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="104"/>
+      <c r="H27" s="104"/>
+      <c r="I27" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="107"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="107"/>
-      <c r="P27" s="107"/>
-      <c r="Q27" s="112"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="106"/>
+      <c r="N27" s="106"/>
+      <c r="O27" s="106"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="111"/>
     </row>
     <row r="28" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
-      <c r="H28" s="105"/>
-      <c r="I28" s="108"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="109"/>
-      <c r="O28" s="109"/>
-      <c r="P28" s="109"/>
-      <c r="Q28" s="113"/>
+      <c r="C28" s="102"/>
+      <c r="D28" s="102"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="104"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="108"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="108"/>
+      <c r="N28" s="108"/>
+      <c r="O28" s="108"/>
+      <c r="P28" s="108"/>
+      <c r="Q28" s="112"/>
     </row>
     <row r="29" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="45"/>
-      <c r="B29" s="115" t="s">
+      <c r="B29" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="115"/>
-      <c r="D29" s="115"/>
-      <c r="E29" s="116"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="117" t="s">
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="115"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="117"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="111"/>
-      <c r="K29" s="111"/>
-      <c r="L29" s="111"/>
-      <c r="M29" s="111"/>
-      <c r="N29" s="111"/>
-      <c r="O29" s="111"/>
-      <c r="P29" s="111"/>
-      <c r="Q29" s="114"/>
+      <c r="H29" s="116"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="110"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="113"/>
     </row>
     <row r="30" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20"/>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
-      <c r="M30" s="83"/>
-      <c r="N30" s="83"/>
-      <c r="O30" s="83"/>
-      <c r="P30" s="83"/>
-      <c r="Q30" s="101"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="100"/>
     </row>
     <row r="31" spans="1:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="118" t="s">
+      <c r="A31" s="117" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="119"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="119"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="119"/>
-      <c r="J31" s="119"/>
-      <c r="K31" s="119"/>
-      <c r="L31" s="119"/>
-      <c r="M31" s="119"/>
-      <c r="N31" s="119"/>
-      <c r="O31" s="119"/>
-      <c r="P31" s="119"/>
-      <c r="Q31" s="120"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="118"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="118"/>
+      <c r="L31" s="118"/>
+      <c r="M31" s="118"/>
+      <c r="N31" s="118"/>
+      <c r="O31" s="118"/>
+      <c r="P31" s="118"/>
+      <c r="Q31" s="119"/>
     </row>
     <row r="32" spans="1:21" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="99"/>
-      <c r="F32" s="99"/>
-      <c r="G32" s="99"/>
-      <c r="H32" s="99"/>
-      <c r="I32" s="99"/>
-      <c r="J32" s="99"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="99"/>
-      <c r="M32" s="99"/>
-      <c r="N32" s="99"/>
-      <c r="O32" s="99"/>
-      <c r="P32" s="99"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="98"/>
+      <c r="O32" s="98"/>
+      <c r="P32" s="98"/>
       <c r="Q32" s="73"/>
     </row>
     <row r="33" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
-      <c r="F33" s="99"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="99"/>
-      <c r="J33" s="99"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="99"/>
-      <c r="M33" s="99"/>
-      <c r="N33" s="99"/>
-      <c r="O33" s="99"/>
-      <c r="P33" s="99"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="98"/>
+      <c r="H33" s="98"/>
+      <c r="I33" s="98"/>
+      <c r="J33" s="98"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="98"/>
+      <c r="N33" s="98"/>
+      <c r="O33" s="98"/>
+      <c r="P33" s="98"/>
       <c r="Q33" s="73"/>
       <c r="R33" s="71"/>
-      <c r="S33" s="82"/>
-      <c r="T33" s="82"/>
-      <c r="U33" s="82"/>
-      <c r="V33" s="82"/>
-      <c r="W33" s="82"/>
-      <c r="X33" s="82"/>
-      <c r="Y33" s="82"/>
-      <c r="Z33" s="82"/>
-      <c r="AA33" s="82"/>
-      <c r="AB33" s="82"/>
-      <c r="AC33" s="82"/>
-      <c r="AD33" s="82"/>
-      <c r="AE33" s="82"/>
-      <c r="AF33" s="82"/>
-      <c r="AG33" s="82"/>
+      <c r="S33" s="81"/>
+      <c r="T33" s="81"/>
+      <c r="U33" s="81"/>
+      <c r="V33" s="81"/>
+      <c r="W33" s="81"/>
+      <c r="X33" s="81"/>
+      <c r="Y33" s="81"/>
+      <c r="Z33" s="81"/>
+      <c r="AA33" s="81"/>
+      <c r="AB33" s="81"/>
+      <c r="AC33" s="81"/>
+      <c r="AD33" s="81"/>
+      <c r="AE33" s="81"/>
+      <c r="AF33" s="81"/>
+      <c r="AG33" s="81"/>
       <c r="AH33" s="71"/>
     </row>
     <row r="34" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="99"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="99"/>
-      <c r="M34" s="99"/>
-      <c r="N34" s="99"/>
-      <c r="O34" s="99"/>
-      <c r="P34" s="99"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="98"/>
+      <c r="L34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+      <c r="O34" s="98"/>
+      <c r="P34" s="98"/>
       <c r="Q34" s="73"/>
       <c r="R34" s="71"/>
-      <c r="S34" s="82"/>
-      <c r="T34" s="82"/>
-      <c r="U34" s="82"/>
-      <c r="V34" s="82"/>
-      <c r="W34" s="82"/>
-      <c r="X34" s="82"/>
-      <c r="Y34" s="82"/>
-      <c r="Z34" s="82"/>
-      <c r="AA34" s="82"/>
-      <c r="AB34" s="82"/>
-      <c r="AC34" s="82"/>
-      <c r="AD34" s="82"/>
-      <c r="AE34" s="82"/>
-      <c r="AF34" s="82"/>
-      <c r="AG34" s="82"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
+      <c r="U34" s="81"/>
+      <c r="V34" s="81"/>
+      <c r="W34" s="81"/>
+      <c r="X34" s="81"/>
+      <c r="Y34" s="81"/>
+      <c r="Z34" s="81"/>
+      <c r="AA34" s="81"/>
+      <c r="AB34" s="81"/>
+      <c r="AC34" s="81"/>
+      <c r="AD34" s="81"/>
+      <c r="AE34" s="81"/>
+      <c r="AF34" s="81"/>
+      <c r="AG34" s="81"/>
       <c r="AH34" s="71"/>
     </row>
     <row r="35" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="99"/>
-      <c r="F35" s="99"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="99"/>
-      <c r="I35" s="99"/>
-      <c r="J35" s="99"/>
-      <c r="K35" s="99"/>
-      <c r="L35" s="99"/>
-      <c r="M35" s="99"/>
-      <c r="N35" s="99"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="98"/>
+      <c r="K35" s="98"/>
+      <c r="L35" s="98"/>
+      <c r="M35" s="98"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="98"/>
+      <c r="P35" s="98"/>
       <c r="Q35" s="73"/>
       <c r="R35" s="71"/>
-      <c r="S35" s="82"/>
-      <c r="T35" s="82"/>
-      <c r="U35" s="82"/>
-      <c r="V35" s="82"/>
-      <c r="W35" s="82"/>
-      <c r="X35" s="82"/>
-      <c r="Y35" s="82"/>
-      <c r="Z35" s="82"/>
-      <c r="AA35" s="82"/>
-      <c r="AB35" s="82"/>
-      <c r="AC35" s="82"/>
-      <c r="AD35" s="82"/>
-      <c r="AE35" s="82"/>
-      <c r="AF35" s="82"/>
-      <c r="AG35" s="82"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
+      <c r="U35" s="81"/>
+      <c r="V35" s="81"/>
+      <c r="W35" s="81"/>
+      <c r="X35" s="81"/>
+      <c r="Y35" s="81"/>
+      <c r="Z35" s="81"/>
+      <c r="AA35" s="81"/>
+      <c r="AB35" s="81"/>
+      <c r="AC35" s="81"/>
+      <c r="AD35" s="81"/>
+      <c r="AE35" s="81"/>
+      <c r="AF35" s="81"/>
+      <c r="AG35" s="81"/>
       <c r="AH35" s="71"/>
     </row>
     <row r="36" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="99"/>
-      <c r="H36" s="99"/>
-      <c r="I36" s="99"/>
-      <c r="J36" s="99"/>
-      <c r="K36" s="99"/>
-      <c r="L36" s="99"/>
-      <c r="M36" s="99"/>
-      <c r="N36" s="99"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="99"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="98"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="98"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="98"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="98"/>
+      <c r="O36" s="98"/>
+      <c r="P36" s="98"/>
       <c r="Q36" s="73"/>
       <c r="R36" s="71"/>
-      <c r="S36" s="82"/>
-      <c r="T36" s="82"/>
-      <c r="U36" s="82"/>
-      <c r="V36" s="82"/>
-      <c r="W36" s="82"/>
-      <c r="X36" s="82"/>
-      <c r="Y36" s="82"/>
-      <c r="Z36" s="82"/>
-      <c r="AA36" s="82"/>
-      <c r="AB36" s="82"/>
-      <c r="AC36" s="82"/>
-      <c r="AD36" s="82"/>
-      <c r="AE36" s="82"/>
-      <c r="AF36" s="82"/>
-      <c r="AG36" s="82"/>
+      <c r="S36" s="81"/>
+      <c r="T36" s="81"/>
+      <c r="U36" s="81"/>
+      <c r="V36" s="81"/>
+      <c r="W36" s="81"/>
+      <c r="X36" s="81"/>
+      <c r="Y36" s="81"/>
+      <c r="Z36" s="81"/>
+      <c r="AA36" s="81"/>
+      <c r="AB36" s="81"/>
+      <c r="AC36" s="81"/>
+      <c r="AD36" s="81"/>
+      <c r="AE36" s="81"/>
+      <c r="AF36" s="81"/>
+      <c r="AG36" s="81"/>
       <c r="AH36" s="71"/>
     </row>
     <row r="37" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="100"/>
-      <c r="G37" s="100"/>
-      <c r="H37" s="100"/>
-      <c r="I37" s="100"/>
-      <c r="J37" s="100"/>
-      <c r="K37" s="100"/>
-      <c r="L37" s="100"/>
-      <c r="M37" s="100"/>
-      <c r="N37" s="100"/>
-      <c r="O37" s="100"/>
-      <c r="P37" s="100"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="99"/>
+      <c r="F37" s="99"/>
+      <c r="G37" s="99"/>
+      <c r="H37" s="99"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="99"/>
+      <c r="K37" s="99"/>
+      <c r="L37" s="99"/>
+      <c r="M37" s="99"/>
+      <c r="N37" s="99"/>
+      <c r="O37" s="99"/>
+      <c r="P37" s="99"/>
       <c r="Q37" s="73"/>
       <c r="R37" s="71"/>
-      <c r="S37" s="82"/>
-      <c r="T37" s="82"/>
-      <c r="U37" s="82"/>
-      <c r="V37" s="82"/>
-      <c r="W37" s="82"/>
-      <c r="X37" s="82"/>
-      <c r="Y37" s="82"/>
-      <c r="Z37" s="82"/>
-      <c r="AA37" s="82"/>
-      <c r="AB37" s="82"/>
-      <c r="AC37" s="82"/>
-      <c r="AD37" s="82"/>
-      <c r="AE37" s="82"/>
-      <c r="AF37" s="82"/>
-      <c r="AG37" s="82"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="81"/>
+      <c r="U37" s="81"/>
+      <c r="V37" s="81"/>
+      <c r="W37" s="81"/>
+      <c r="X37" s="81"/>
+      <c r="Y37" s="81"/>
+      <c r="Z37" s="81"/>
+      <c r="AA37" s="81"/>
+      <c r="AB37" s="81"/>
+      <c r="AC37" s="81"/>
+      <c r="AD37" s="81"/>
+      <c r="AE37" s="81"/>
+      <c r="AF37" s="81"/>
+      <c r="AG37" s="81"/>
       <c r="AH37" s="71"/>
     </row>
     <row r="38" spans="1:34" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,23 +2631,23 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="83" t="s">
+      <c r="B39" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="83"/>
-      <c r="D39" s="83"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="83"/>
-      <c r="G39" s="83"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="83"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="83"/>
-      <c r="M39" s="83"/>
-      <c r="N39" s="83"/>
-      <c r="O39" s="83"/>
-      <c r="P39" s="83"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="82"/>
+      <c r="N39" s="82"/>
+      <c r="O39" s="82"/>
+      <c r="P39" s="82"/>
       <c r="Q39" s="70"/>
       <c r="R39" s="71"/>
       <c r="S39" s="71"/>
@@ -2675,20 +2669,20 @@
     </row>
     <row r="40" spans="1:34" ht="3.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="86"/>
-      <c r="D40" s="86"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="86"/>
-      <c r="G40" s="86"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="85"/>
       <c r="H40" s="49"/>
-      <c r="I40" s="89" t="s">
+      <c r="I40" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="J40" s="90"/>
-      <c r="K40" s="90"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="89"/>
       <c r="L40" s="49"/>
       <c r="M40" s="49"/>
       <c r="N40" s="49"/>
@@ -2698,16 +2692,16 @@
     </row>
     <row r="41" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="51"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="87"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
+      <c r="B41" s="84"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="86"/>
       <c r="H41" s="4"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="92"/>
-      <c r="K41" s="92"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="91"/>
+      <c r="K41" s="91"/>
       <c r="L41" s="52"/>
       <c r="M41" s="52"/>
       <c r="N41" s="52"/>
@@ -2717,12 +2711,12 @@
     </row>
     <row r="42" spans="1:34" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
-      <c r="B42" s="85"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="88"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
       <c r="H42" s="4"/>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
@@ -2752,35 +2746,35 @@
       <c r="O43" s="58"/>
       <c r="P43" s="58"/>
       <c r="Q43" s="56"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="94"/>
-      <c r="T43" s="94"/>
-      <c r="U43" s="94"/>
+      <c r="R43" s="92"/>
+      <c r="S43" s="93"/>
+      <c r="T43" s="93"/>
+      <c r="U43" s="93"/>
     </row>
     <row r="44" spans="1:34" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="59"/>
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="C44" s="92"/>
-      <c r="D44" s="95"/>
-      <c r="E44" s="95"/>
-      <c r="F44" s="95"/>
-      <c r="G44" s="95"/>
-      <c r="H44" s="96"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="98"/>
-      <c r="K44" s="98"/>
-      <c r="L44" s="98"/>
-      <c r="M44" s="98"/>
-      <c r="N44" s="98"/>
-      <c r="O44" s="80"/>
-      <c r="P44" s="80"/>
-      <c r="Q44" s="81"/>
-      <c r="R44" s="93"/>
-      <c r="S44" s="94"/>
-      <c r="T44" s="94"/>
-      <c r="U44" s="94"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="94"/>
+      <c r="E44" s="94"/>
+      <c r="F44" s="94"/>
+      <c r="G44" s="94"/>
+      <c r="H44" s="95"/>
+      <c r="I44" s="96"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
+      <c r="M44" s="97"/>
+      <c r="N44" s="97"/>
+      <c r="O44" s="79"/>
+      <c r="P44" s="79"/>
+      <c r="Q44" s="80"/>
+      <c r="R44" s="92"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
     </row>
     <row r="45" spans="1:34" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
@@ -2788,101 +2782,101 @@
       <c r="C45" s="60"/>
       <c r="D45" s="61"/>
       <c r="E45" s="61"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
+      <c r="F45" s="77"/>
+      <c r="G45" s="77"/>
+      <c r="H45" s="77"/>
       <c r="I45" s="62"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
+      <c r="J45" s="78"/>
+      <c r="K45" s="78"/>
+      <c r="L45" s="78"/>
+      <c r="M45" s="78"/>
       <c r="N45" s="63"/>
-      <c r="O45" s="80"/>
-      <c r="P45" s="80"/>
-      <c r="Q45" s="81"/>
+      <c r="O45" s="79"/>
+      <c r="P45" s="79"/>
+      <c r="Q45" s="80"/>
     </row>
     <row r="46" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="59"/>
-      <c r="B46" s="149" t="s">
+      <c r="B46" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="154"/>
-      <c r="D46" s="154"/>
-      <c r="E46" s="154"/>
-      <c r="F46" s="154"/>
-      <c r="G46" s="154"/>
-      <c r="H46" s="155"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="149"/>
+      <c r="E46" s="149"/>
+      <c r="F46" s="149"/>
+      <c r="G46" s="149"/>
+      <c r="H46" s="95"/>
       <c r="I46" s="152" t="s">
         <v>31</v>
       </c>
       <c r="J46" s="152"/>
-      <c r="K46" s="153"/>
-      <c r="L46" s="153"/>
-      <c r="M46" s="153"/>
-      <c r="N46" s="153"/>
-      <c r="O46" s="153"/>
-      <c r="P46" s="153"/>
+      <c r="K46" s="149"/>
+      <c r="L46" s="149"/>
+      <c r="M46" s="149"/>
+      <c r="N46" s="149"/>
+      <c r="O46" s="149"/>
+      <c r="P46" s="149"/>
       <c r="Q46" s="64"/>
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="59"/>
-      <c r="B47" s="149"/>
-      <c r="C47" s="153"/>
-      <c r="D47" s="153"/>
-      <c r="E47" s="153"/>
-      <c r="F47" s="153"/>
-      <c r="G47" s="153"/>
-      <c r="H47" s="96"/>
-      <c r="I47" s="151"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="149"/>
+      <c r="D47" s="149"/>
+      <c r="E47" s="149"/>
+      <c r="F47" s="149"/>
+      <c r="G47" s="149"/>
+      <c r="H47" s="95"/>
+      <c r="I47" s="153"/>
       <c r="J47" s="152"/>
-      <c r="K47" s="153"/>
-      <c r="L47" s="153"/>
-      <c r="M47" s="153"/>
-      <c r="N47" s="153"/>
-      <c r="O47" s="153"/>
-      <c r="P47" s="153"/>
+      <c r="K47" s="149"/>
+      <c r="L47" s="149"/>
+      <c r="M47" s="149"/>
+      <c r="N47" s="149"/>
+      <c r="O47" s="149"/>
+      <c r="P47" s="149"/>
       <c r="Q47" s="75"/>
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="59"/>
-      <c r="B48" s="149"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
-      <c r="F48" s="76"/>
-      <c r="G48" s="76"/>
-      <c r="H48" s="150"/>
-      <c r="I48" s="151"/>
+      <c r="B48" s="148"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="150"/>
+      <c r="E48" s="150"/>
+      <c r="F48" s="150"/>
+      <c r="G48" s="150"/>
+      <c r="H48" s="151"/>
+      <c r="I48" s="153"/>
       <c r="J48" s="152"/>
-      <c r="K48" s="76"/>
-      <c r="L48" s="76"/>
-      <c r="M48" s="76"/>
-      <c r="N48" s="76"/>
-      <c r="O48" s="76"/>
-      <c r="P48" s="76"/>
+      <c r="K48" s="150"/>
+      <c r="L48" s="150"/>
+      <c r="M48" s="150"/>
+      <c r="N48" s="150"/>
+      <c r="O48" s="150"/>
+      <c r="P48" s="150"/>
       <c r="Q48" s="75"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="65"/>
       <c r="B49" s="66"/>
-      <c r="C49" s="77" t="s">
+      <c r="C49" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="77"/>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="77"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
       <c r="I49" s="67"/>
       <c r="J49" s="68"/>
-      <c r="K49" s="77" t="s">
+      <c r="K49" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="L49" s="77"/>
-      <c r="M49" s="77"/>
-      <c r="N49" s="77"/>
-      <c r="O49" s="77"/>
-      <c r="P49" s="77"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="76"/>
+      <c r="O49" s="76"/>
+      <c r="P49" s="76"/>
       <c r="Q49" s="69"/>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -2912,6 +2906,8 @@
     <mergeCell ref="I46:J48"/>
     <mergeCell ref="K48:P48"/>
     <mergeCell ref="K47:P47"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="K46:P46"/>
     <mergeCell ref="D1:Q1"/>
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="D3:Q3"/>
@@ -2945,14 +2941,14 @@
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="P16:Q16"/>
     <mergeCell ref="B18:P19"/>
+    <mergeCell ref="B30:Q30"/>
+    <mergeCell ref="A31:Q31"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="H22:J22"/>
     <mergeCell ref="K22:P22"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:P23"/>
-    <mergeCell ref="S36:AG36"/>
-    <mergeCell ref="S33:AG33"/>
     <mergeCell ref="B25:Q25"/>
     <mergeCell ref="E26:P26"/>
     <mergeCell ref="B27:D27"/>
@@ -2964,28 +2960,26 @@
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B30:Q30"/>
-    <mergeCell ref="A31:Q31"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="O45:Q45"/>
+    <mergeCell ref="R43:U44"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="I44:N44"/>
+    <mergeCell ref="O44:Q44"/>
     <mergeCell ref="S37:AG37"/>
     <mergeCell ref="B39:P39"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:G42"/>
     <mergeCell ref="I40:K41"/>
-    <mergeCell ref="R43:U44"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="I44:N44"/>
-    <mergeCell ref="O44:Q44"/>
     <mergeCell ref="B32:P37"/>
     <mergeCell ref="S34:AG34"/>
     <mergeCell ref="S35:AG35"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="K46:P46"/>
+    <mergeCell ref="S36:AG36"/>
+    <mergeCell ref="S33:AG33"/>
     <mergeCell ref="C49:H49"/>
     <mergeCell ref="K49:P49"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="O45:Q45"/>
   </mergeCells>
   <pageMargins left="0.9055118110236221" right="0.31496062992125984" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
@@ -2994,15 +2988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D262036FF67A5D43BF6E290DEB360352" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c503d2a7b448377a6cc9e75158e3af5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4e744003-367c-4be8-bc40-2385cb622540" xmlns:ns3="0930cf9b-719b-4120-8db4-f84070340397" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9cea96fa3cc1abdf61d90e2bf9fac8d2" ns2:_="" ns3:_="">
     <xsd:import namespace="4e744003-367c-4be8-bc40-2385cb622540"/>
@@ -3219,21 +3204,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3DC5811-E2D9-4774-B143-A47CE40C3F55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3252,7 +3238,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CEBEA7B-59B1-46CE-A437-47DAA38AB618}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3267,4 +3253,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90864A59-6AB3-4A4B-906C-17AADC78847C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>